<commit_message>
refactor: update kalman algo and merge with PID
</commit_message>
<xml_diff>
--- a/Ultrasonic + Accelerometer/pico_accelerator/Documentation/algo_performance.xlsx
+++ b/Ultrasonic + Accelerometer/pico_accelerator/Documentation/algo_performance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\CSC2003-B1\Ultrasonic + Accelerometer\pico_accelerator\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4E6C37-42F5-4217-BFA9-3257B8984E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8426E147-51F0-46DC-AD8B-89CC042801FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B3ABCD8F-5EFA-4CD1-BF4C-BA51D83D907B}"/>
   </bookViews>
@@ -138,13 +138,13 @@
     <t>ky angle1.85</t>
   </si>
   <si>
-    <t>complementary filter (Y-axis)</t>
-  </si>
-  <si>
-    <t>Kalman filter (Y-axis)</t>
-  </si>
-  <si>
     <t>Raw Data</t>
+  </si>
+  <si>
+    <t>Kalman filter (Y-angle)</t>
+  </si>
+  <si>
+    <t>complementary filter (Y-angle)</t>
   </si>
 </sst>
 </file>
@@ -264,7 +264,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>complementary filter (Y-axis)</c:v>
+                  <c:v>complementary filter (Y-angle)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -357,7 +357,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Kalman filter (Y-axis)</c:v>
+                  <c:v>Kalman filter (Y-angle)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1546,7 +1546,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -1729,19 +1729,19 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>35</v>

</xml_diff>